<commit_message>
Namen verander naar engels
</commit_message>
<xml_diff>
--- a/Dashboard/Data/Verkoop per brandstof (België) met market share.xlsx
+++ b/Dashboard/Data/Verkoop per brandstof (België) met market share.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroh\OneDrive - Universiteit Hasselt\2020-2021\Business intelligence\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroh\OneDrive - Universiteit Hasselt\2020-2021\Business intelligence\Project\BUSIN\Dashboard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27D47D1-DDAC-4681-811E-0AE8377D7B0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9359553-7110-4D15-B709-D3B02F530FFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7174A03F-5037-4A99-A745-0BAFCEFC424E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7174A03F-5037-4A99-A745-0BAFCEFC424E}"/>
   </bookViews>
   <sheets>
     <sheet name="Nieuw" sheetId="1" r:id="rId1"/>
@@ -35,57 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>Fuel</t>
   </si>
   <si>
-    <t>onbekend</t>
-  </si>
-  <si>
-    <t>benzine</t>
-  </si>
-  <si>
-    <t>diesel</t>
-  </si>
-  <si>
-    <t>gas + benzine</t>
-  </si>
-  <si>
-    <t>elektrisch</t>
-  </si>
-  <si>
-    <t>andere</t>
-  </si>
-  <si>
-    <t>aardgas</t>
-  </si>
-  <si>
-    <t>benzine + elektrisch</t>
-  </si>
-  <si>
-    <t>diesel+elektrisch</t>
-  </si>
-  <si>
     <t>mengsmering</t>
-  </si>
-  <si>
-    <t>waterstof</t>
-  </si>
-  <si>
-    <t>diesel + gas</t>
-  </si>
-  <si>
-    <t>elektrisch + lpg</t>
-  </si>
-  <si>
-    <t>bio-ethanol</t>
-  </si>
-  <si>
-    <t>waterstof + elektrisch</t>
-  </si>
-  <si>
-    <t>benzine + aardgas</t>
   </si>
   <si>
     <t>MS12</t>
@@ -110,6 +65,54 @@
   </si>
   <si>
     <t>MS19</t>
+  </si>
+  <si>
+    <t>Petrol</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>Gas + petrol</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Alternative</t>
+  </si>
+  <si>
+    <t>Natural gas</t>
+  </si>
+  <si>
+    <t>Petrol + electric</t>
+  </si>
+  <si>
+    <t>Diesel+electric</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>Diesel + gas</t>
+  </si>
+  <si>
+    <t>Electric + liquefied petroleum gas</t>
+  </si>
+  <si>
+    <t>Bio-ethanol</t>
+  </si>
+  <si>
+    <t>Hydrogen + electric</t>
+  </si>
+  <si>
+    <t>Petrol + natural gas</t>
+  </si>
+  <si>
+    <t>Diesel + electric</t>
   </si>
 </sst>
 </file>
@@ -502,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79587E2-A047-4539-A758-4FFF904C27F2}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,54 +529,54 @@
         <v>2012</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D1">
         <v>2013</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F1">
         <v>2014</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H1">
         <v>2015</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J1">
         <v>2016</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="L1">
         <v>2017</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="N1">
         <v>2018</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="P1">
         <v>2019</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2">
         <v>40</v>
@@ -634,7 +637,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
         <v>145844</v>
@@ -695,7 +698,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
         <v>339217</v>
@@ -756,7 +759,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>193</v>
@@ -817,7 +820,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2">
         <v>560</v>
@@ -878,7 +881,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -939,7 +942,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2">
         <v>73</v>
@@ -1001,7 +1004,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2">
         <v>4433</v>
@@ -1062,7 +1065,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2">
         <v>326</v>
@@ -1123,7 +1126,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B11" s="2">
         <v>0</v>
@@ -1184,7 +1187,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
@@ -1245,7 +1248,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -1306,7 +1309,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -1367,7 +1370,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2">
         <v>21</v>
@@ -1428,7 +1431,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -1489,7 +1492,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2">
         <v>4</v>
@@ -1561,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E43405-3917-45B8-BB80-10A13342769C}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1585,54 +1588,54 @@
         <v>2012</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D1">
         <v>2013</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F1">
         <v>2014</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H1">
         <v>2015</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J1">
         <v>2016</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="L1">
         <v>2017</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="N1">
         <v>2018</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="P1">
         <v>2019</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2">
         <v>9</v>
@@ -1693,7 +1696,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
         <v>261216</v>
@@ -1754,7 +1757,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
         <v>460185</v>
@@ -1815,7 +1818,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>5214</v>
@@ -1876,7 +1879,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2">
         <v>51</v>
@@ -1937,7 +1940,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2">
         <v>7</v>
@@ -1998,7 +2001,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2">
         <v>16</v>
@@ -2059,7 +2062,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2">
         <v>689</v>
@@ -2120,7 +2123,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2">
         <v>6</v>
@@ -2181,7 +2184,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
@@ -2242,7 +2245,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
@@ -2303,7 +2306,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
@@ -2364,7 +2367,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -2425,7 +2428,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
@@ -2486,7 +2489,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -2547,7 +2550,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2">
         <v>10</v>

</xml_diff>